<commit_message>
Now point of overcoming used modelling noise statistics
</commit_message>
<xml_diff>
--- a/tables/results.xlsx
+++ b/tables/results.xlsx
@@ -778,10 +778,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>302</v>
+        <v>328</v>
       </c>
       <c r="C3" t="n">
-        <v>302</v>
+        <v>328</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -789,10 +789,10 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>302</v>
+        <v>350</v>
       </c>
       <c r="H3" t="n">
-        <v>302</v>
+        <v>350</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>302</v>
+        <v>329</v>
       </c>
       <c r="M3" t="n">
-        <v>302</v>
+        <v>329</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
@@ -811,10 +811,10 @@
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>302</v>
+        <v>327</v>
       </c>
       <c r="R3" t="n">
-        <v>302</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4">
@@ -1077,43 +1077,31 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>302</v>
+        <v>330</v>
       </c>
       <c r="C13" t="n">
-        <v>302</v>
+        <v>330</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
           <t>Point of overcoming</t>
         </is>
       </c>
-      <c r="G13" t="n">
-        <v>302</v>
-      </c>
-      <c r="H13" t="n">
-        <v>302</v>
-      </c>
       <c r="K13" t="inlineStr">
         <is>
           <t>Point of overcoming</t>
         </is>
       </c>
-      <c r="L13" t="n">
-        <v>302</v>
-      </c>
-      <c r="M13" t="n">
-        <v>302</v>
-      </c>
       <c r="P13" t="inlineStr">
         <is>
           <t>Point of overcoming</t>
         </is>
       </c>
       <c r="Q13" t="n">
-        <v>302</v>
+        <v>327</v>
       </c>
       <c r="R13" t="n">
-        <v>302</v>
+        <v>326</v>
       </c>
     </row>
     <row r="14">
@@ -1133,22 +1121,10 @@
           <t>X[Q]</t>
         </is>
       </c>
-      <c r="G14" t="n">
-        <v>3.33066907387547e-16</v>
-      </c>
-      <c r="H14" t="n">
-        <v>3.33066907387547e-16</v>
-      </c>
       <c r="K14" t="inlineStr">
         <is>
           <t>X[Q]</t>
         </is>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>
@@ -1179,22 +1155,10 @@
           <t>X[Q+10]</t>
         </is>
       </c>
-      <c r="G15" t="n">
-        <v>0.003571256655593658</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.003571256655593658</v>
-      </c>
       <c r="K15" t="inlineStr">
         <is>
           <t>X[Q+10]</t>
         </is>
-      </c>
-      <c r="L15" t="n">
-        <v>0.01515598145843722</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0.01515598145843722</v>
       </c>
       <c r="P15" t="inlineStr">
         <is>
@@ -1225,22 +1189,10 @@
           <t>X[Q+20]</t>
         </is>
       </c>
-      <c r="G16" t="n">
-        <v>0.01851874918872343</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.01851874918872343</v>
-      </c>
       <c r="K16" t="inlineStr">
         <is>
           <t>X[Q+20]</t>
         </is>
-      </c>
-      <c r="L16" t="n">
-        <v>0.03153547418523062</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0.03153547418523062</v>
       </c>
       <c r="P16" t="inlineStr">
         <is>
@@ -1271,22 +1223,10 @@
           <t>X[Q+30]</t>
         </is>
       </c>
-      <c r="G17" t="n">
-        <v>0.03610503537199328</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.03610503537199328</v>
-      </c>
       <c r="K17" t="inlineStr">
         <is>
           <t>X[Q+30]</t>
         </is>
-      </c>
-      <c r="L17" t="n">
-        <v>0.03602545401899948</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0.03602545401899948</v>
       </c>
       <c r="P17" t="inlineStr">
         <is>
@@ -1376,43 +1316,31 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>301</v>
+        <v>334</v>
       </c>
       <c r="C23" t="n">
-        <v>301</v>
+        <v>333</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
           <t>Point of overcoming</t>
         </is>
       </c>
-      <c r="G23" t="n">
-        <v>301</v>
-      </c>
-      <c r="H23" t="n">
-        <v>301</v>
-      </c>
       <c r="K23" t="inlineStr">
         <is>
           <t>Point of overcoming</t>
         </is>
       </c>
-      <c r="L23" t="n">
-        <v>301</v>
-      </c>
-      <c r="M23" t="n">
-        <v>301</v>
-      </c>
       <c r="P23" t="inlineStr">
         <is>
           <t>Point of overcoming</t>
         </is>
       </c>
       <c r="Q23" t="n">
-        <v>301</v>
+        <v>332</v>
       </c>
       <c r="R23" t="n">
-        <v>301</v>
+        <v>331</v>
       </c>
     </row>
     <row r="24">
@@ -1432,22 +1360,10 @@
           <t>X[Q]</t>
         </is>
       </c>
-      <c r="G24" t="n">
-        <v>2.86534206772604e-05</v>
-      </c>
-      <c r="H24" t="n">
-        <v>2.86534206772604e-05</v>
-      </c>
       <c r="K24" t="inlineStr">
         <is>
           <t>X[Q]</t>
         </is>
-      </c>
-      <c r="L24" t="n">
-        <v>0.0007233287937621347</v>
-      </c>
-      <c r="M24" t="n">
-        <v>0.0007233287937621347</v>
       </c>
       <c r="P24" t="inlineStr">
         <is>
@@ -1478,22 +1394,10 @@
           <t>X[Q+10]</t>
         </is>
       </c>
-      <c r="G25" t="n">
-        <v>0.00506994762797075</v>
-      </c>
-      <c r="H25" t="n">
-        <v>0.00506994762797075</v>
-      </c>
       <c r="K25" t="inlineStr">
         <is>
           <t>X[Q+10]</t>
         </is>
-      </c>
-      <c r="L25" t="n">
-        <v>0.03444585922870569</v>
-      </c>
-      <c r="M25" t="n">
-        <v>0.03444585922870569</v>
       </c>
       <c r="P25" t="inlineStr">
         <is>
@@ -1524,22 +1428,10 @@
           <t>X[Q+20]</t>
         </is>
       </c>
-      <c r="G26" t="n">
-        <v>0.0302489427173489</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.0302489427173489</v>
-      </c>
       <c r="K26" t="inlineStr">
         <is>
           <t>X[Q+20]</t>
         </is>
-      </c>
-      <c r="L26" t="n">
-        <v>0.09610248649709552</v>
-      </c>
-      <c r="M26" t="n">
-        <v>0.09610248649709552</v>
       </c>
       <c r="P26" t="inlineStr">
         <is>
@@ -1570,22 +1462,10 @@
           <t>X[Q+30]</t>
         </is>
       </c>
-      <c r="G27" t="n">
-        <v>0.08547445816695243</v>
-      </c>
-      <c r="H27" t="n">
-        <v>0.08547445816695243</v>
-      </c>
       <c r="K27" t="inlineStr">
         <is>
           <t>X[Q+30]</t>
         </is>
-      </c>
-      <c r="L27" t="n">
-        <v>0.1507789796678952</v>
-      </c>
-      <c r="M27" t="n">
-        <v>0.1507789796678952</v>
       </c>
       <c r="P27" t="inlineStr">
         <is>
@@ -1675,32 +1555,26 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C33" t="n">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
           <t>Point of overcoming</t>
         </is>
       </c>
-      <c r="G33" t="n">
-        <v>302</v>
-      </c>
-      <c r="H33" t="n">
-        <v>302</v>
-      </c>
       <c r="K33" t="inlineStr">
         <is>
           <t>Point of overcoming</t>
         </is>
       </c>
       <c r="L33" t="n">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="M33" t="n">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="P33" t="inlineStr">
         <is>
@@ -1708,10 +1582,10 @@
         </is>
       </c>
       <c r="Q33" t="n">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="R33" t="n">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34">
@@ -1731,12 +1605,6 @@
           <t>X[Q]</t>
         </is>
       </c>
-      <c r="G34" t="n">
-        <v>2.220446049250313e-16</v>
-      </c>
-      <c r="H34" t="n">
-        <v>2.220446049250313e-16</v>
-      </c>
       <c r="K34" t="inlineStr">
         <is>
           <t>X[Q]</t>
@@ -1777,12 +1645,6 @@
           <t>X[Q+10]</t>
         </is>
       </c>
-      <c r="G35" t="n">
-        <v>0.03600000043698748</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0.03600000043698748</v>
-      </c>
       <c r="K35" t="inlineStr">
         <is>
           <t>X[Q+10]</t>
@@ -1823,12 +1685,6 @@
           <t>X[Q+20]</t>
         </is>
       </c>
-      <c r="G36" t="n">
-        <v>0.03993265723796668</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0.03993265723796668</v>
-      </c>
       <c r="K36" t="inlineStr">
         <is>
           <t>X[Q+20]</t>
@@ -1868,12 +1724,6 @@
         <is>
           <t>X[Q+30]</t>
         </is>
-      </c>
-      <c r="G37" t="n">
-        <v>0.03185894778150467</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0.03185894778150467</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Testing of new approach reworked (report and timeTests.ipynb)
</commit_message>
<xml_diff>
--- a/tables/results.xlsx
+++ b/tables/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\ivank\Documents\Education\magistracy\ResearchWork\code\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\ivank\Documents\Education\magistracy\ResearchWork\researchWork\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259825B2-F87D-487F-A71F-3D91C667847B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921E9969-1273-40F1-9C03-424E8CBE1A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelling" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="26">
   <si>
     <t>Permanent</t>
   </si>
@@ -82,6 +82,24 @@
   </si>
   <si>
     <t>Num Points of overcoming</t>
+  </si>
+  <si>
+    <t>permanent</t>
+  </si>
+  <si>
+    <t>HeterType</t>
+  </si>
+  <si>
+    <t>StatType</t>
+  </si>
+  <si>
+    <t>temporary</t>
+  </si>
+  <si>
+    <t>shifted</t>
+  </si>
+  <si>
+    <t>outlier</t>
   </si>
 </sst>
 </file>
@@ -427,15 +445,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:E15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,8 +475,41 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -468,8 +525,41 @@
       <c r="E2">
         <v>0.21845603181440629</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <v>0.23910427385415439</v>
+      </c>
+      <c r="L2">
+        <v>0.20623982447355849</v>
+      </c>
+      <c r="M2">
+        <v>0.2339014764166682</v>
+      </c>
+      <c r="N2">
+        <v>0.21845603181440629</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2">
+        <v>0.23910427385415439</v>
+      </c>
+      <c r="T2">
+        <v>0.20623982447355849</v>
+      </c>
+      <c r="U2">
+        <v>0.2339014764166682</v>
+      </c>
+      <c r="V2">
+        <v>0.21845603181440629</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -485,8 +575,61 @@
       <c r="E3">
         <v>0.2167079398816309</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>0.23522107691293209</v>
+      </c>
+      <c r="L3">
+        <v>0.20543257450812</v>
+      </c>
+      <c r="M3">
+        <v>0.2297395892421695</v>
+      </c>
+      <c r="N3">
+        <v>0.2167079398816309</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>6.8502538801477234E-2</v>
+      </c>
+      <c r="T3">
+        <v>5.9271344505759327E-2</v>
+      </c>
+      <c r="U3">
+        <v>6.6945560445144991E-2</v>
+      </c>
+      <c r="V3">
+        <v>6.2381656410886721E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <v>0.237174526731387</v>
+      </c>
+      <c r="T4">
+        <v>0.20436129012957929</v>
+      </c>
+      <c r="U4">
+        <v>0.23190675646389119</v>
+      </c>
+      <c r="V4">
+        <v>0.21658562073538301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -502,8 +645,41 @@
       <c r="E5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S5">
+        <v>0.23360443459936939</v>
+      </c>
+      <c r="T5">
+        <v>0.20690478595875239</v>
+      </c>
+      <c r="U5">
+        <v>0.2286934212741393</v>
+      </c>
+      <c r="V5">
+        <v>0.21612047059277359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -519,8 +695,23 @@
       <c r="E6">
         <v>6.2381656410886721E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>6.8502538801477234E-2</v>
+      </c>
+      <c r="L6">
+        <v>5.9271344505759327E-2</v>
+      </c>
+      <c r="M6">
+        <v>6.6945560445144991E-2</v>
+      </c>
+      <c r="N6">
+        <v>6.2381656410886721E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -536,8 +727,43 @@
       <c r="E7">
         <v>6.1582231192767539E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>6.7345506222796128E-2</v>
+      </c>
+      <c r="L7">
+        <v>5.9055195274466933E-2</v>
+      </c>
+      <c r="M7">
+        <v>6.5679226981861863E-2</v>
+      </c>
+      <c r="N7">
+        <v>6.1582231192767539E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q8" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" t="s">
+        <v>6</v>
+      </c>
+      <c r="S8">
+        <v>0.23522107691293209</v>
+      </c>
+      <c r="T8">
+        <v>0.20543257450812</v>
+      </c>
+      <c r="U8">
+        <v>0.2297395892421695</v>
+      </c>
+      <c r="V8">
+        <v>0.2167079398816309</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -553,8 +779,41 @@
       <c r="E9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>23</v>
+      </c>
+      <c r="R9" t="s">
+        <v>6</v>
+      </c>
+      <c r="S9">
+        <v>6.7345506222796128E-2</v>
+      </c>
+      <c r="T9">
+        <v>5.9055195274466933E-2</v>
+      </c>
+      <c r="U9">
+        <v>6.5679226981861863E-2</v>
+      </c>
+      <c r="V9">
+        <v>6.1582231192767539E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -570,8 +829,41 @@
       <c r="E10">
         <v>0.21658562073538301</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>0.237174526731387</v>
+      </c>
+      <c r="L10">
+        <v>0.20436129012957929</v>
+      </c>
+      <c r="M10">
+        <v>0.23190675646389119</v>
+      </c>
+      <c r="N10">
+        <v>0.21658562073538301</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>24</v>
+      </c>
+      <c r="R10" t="s">
+        <v>6</v>
+      </c>
+      <c r="S10">
+        <v>0.2335827249185832</v>
+      </c>
+      <c r="T10">
+        <v>0.2035613248694968</v>
+      </c>
+      <c r="U10">
+        <v>0.2279274205230947</v>
+      </c>
+      <c r="V10">
+        <v>0.21429840603833969</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -587,8 +879,41 @@
       <c r="E11">
         <v>0.21429840603833969</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>0.2335827249185832</v>
+      </c>
+      <c r="L11">
+        <v>0.2035613248694968</v>
+      </c>
+      <c r="M11">
+        <v>0.2279274205230947</v>
+      </c>
+      <c r="N11">
+        <v>0.21429840603833969</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>25</v>
+      </c>
+      <c r="R11" t="s">
+        <v>6</v>
+      </c>
+      <c r="S11">
+        <v>0.23067557843651321</v>
+      </c>
+      <c r="T11">
+        <v>0.2061419970371397</v>
+      </c>
+      <c r="U11">
+        <v>0.2254137170323581</v>
+      </c>
+      <c r="V11">
+        <v>0.21387926387315609</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -604,8 +929,23 @@
       <c r="E13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -621,8 +961,23 @@
       <c r="E14">
         <v>0.21612047059277359</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>0.23360443459936939</v>
+      </c>
+      <c r="L14">
+        <v>0.20690478595875239</v>
+      </c>
+      <c r="M14">
+        <v>0.2286934212741393</v>
+      </c>
+      <c r="N14">
+        <v>0.21612047059277359</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -636,6 +991,21 @@
         <v>0.2254137170323581</v>
       </c>
       <c r="E15">
+        <v>0.21387926387315609</v>
+      </c>
+      <c r="J15" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15">
+        <v>0.23067557843651321</v>
+      </c>
+      <c r="L15">
+        <v>0.2061419970371397</v>
+      </c>
+      <c r="M15">
+        <v>0.2254137170323581</v>
+      </c>
+      <c r="N15">
         <v>0.21387926387315609</v>
       </c>
     </row>
@@ -1450,7 +1820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AM38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="Q61" sqref="Q61"/>
     </sheetView>
   </sheetViews>

</xml_diff>